<commit_message>
Creación de programa para Atica y ajustes en la sociedad
</commit_message>
<xml_diff>
--- a/OutputFiles/AGOSTO 2025.xlsx
+++ b/OutputFiles/AGOSTO 2025.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://jtccomco-my.sharepoint.com/personal/alan_bohorquez_jtc_com_co/Documents/Escritorio/Alan/Python Projects/OutputFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{AF2CDF3E-9010-482B-B671-E6697FB47653}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A3CBC8C7-D938-4388-99C1-2C2DD0B15E7C}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{AF2CDF3E-9010-482B-B671-E6697FB47653}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4FC7F11F-6613-4033-8397-DC5FE501EAAD}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>

</xml_diff>